<commit_message>
+hist for outdoor experiment; problem needed to be explained
</commit_message>
<xml_diff>
--- a/communicate_with_basis_station_in_matlab/calibrations/outdoor/OUTDOOR_MEASUREMENT_07_27_2017/outdoor_calibration_results.xlsx
+++ b/communicate_with_basis_station_in_matlab/calibrations/outdoor/OUTDOOR_MEASUREMENT_07_27_2017/outdoor_calibration_results.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yitong\GitHub\thesis_indoorLocalization\communicate_with_basis_station_in_matlab\calibrations\outdoor\OUTDOOR_MEASUREMENT_07_27_2017\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="14295" windowHeight="12630" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="12630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="38">
   <si>
     <t>x</t>
   </si>
@@ -311,18 +316,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -332,7 +331,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -341,150 +340,6 @@
       <color rgb="FF005CC5"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -499,7 +354,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,7 +369,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799951170384838"/>
+        <fgColor theme="4" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +381,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799951170384838"/>
+        <fgColor theme="7" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,194 +397,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -767,251 +436,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1036,61 +463,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1139,7 +522,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1174,7 +557,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1377,31 +760,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="13.8583333333333" customWidth="1"/>
-    <col min="6" max="6" width="12.5666666666667"/>
-    <col min="11" max="12" width="12.5666666666667"/>
-    <col min="14" max="16" width="12.5666666666667"/>
-    <col min="17" max="17" width="11.425"/>
-    <col min="20" max="20" width="12.5666666666667"/>
-    <col min="23" max="23" width="12.5666666666667"/>
-    <col min="26" max="26" width="9.14166666666667" style="13"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125"/>
+    <col min="11" max="12" width="12.5703125"/>
+    <col min="14" max="16" width="12.5703125"/>
+    <col min="17" max="17" width="11.42578125"/>
+    <col min="20" max="20" width="12.5703125"/>
+    <col min="23" max="23" width="12.5703125"/>
+    <col min="26" max="26" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:23">
+    <row r="1" spans="2:26">
       <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1427,7 +810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:24">
+    <row r="2" spans="2:26">
       <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="14.25" spans="2:26">
+    <row r="3" spans="2:26">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -1486,7 +869,7 @@
         <v>236.363636363636</v>
       </c>
       <c r="F3">
-        <v>4.37632135306554</v>
+        <v>4.3763213530655403</v>
       </c>
       <c r="K3">
         <v>491.787234042553</v>
@@ -1498,16 +881,16 @@
         <v>712.28</v>
       </c>
       <c r="R3">
-        <v>36.0433333333333</v>
+        <v>36.043333333333301</v>
       </c>
       <c r="T3">
-        <v>918.823529411765</v>
+        <v>918.82352941176498</v>
       </c>
       <c r="U3">
-        <v>62.5294117647059</v>
+        <v>62.529411764705898</v>
       </c>
       <c r="W3">
-        <v>1180.66666666667</v>
+        <v>1180.6666666666699</v>
       </c>
       <c r="X3">
         <v>24.3333333333333</v>
@@ -1516,7 +899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" ht="62.25" spans="3:26">
+    <row r="4" spans="2:26" ht="76.5">
       <c r="C4" t="s">
         <v>14</v>
       </c>
@@ -1524,16 +907,16 @@
         <v>15</v>
       </c>
       <c r="E4" s="15">
-        <v>2.4339409209068</v>
+        <v>2.4339409209067999</v>
       </c>
       <c r="K4">
-        <v>5.00747842864033</v>
+        <v>5.0074784286403302</v>
       </c>
       <c r="Q4">
-        <v>7.22906801007557</v>
+        <v>7.2290680100755704</v>
       </c>
       <c r="T4">
-        <v>9.31011112757446</v>
+        <v>9.3101111275744604</v>
       </c>
       <c r="W4">
         <v>11.9483291351806</v>
@@ -1542,7 +925,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" ht="14.25" spans="2:15">
+    <row r="6" spans="2:26">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -1553,13 +936,13 @@
         <v>311.767441860465</v>
       </c>
       <c r="F6">
-        <v>49.2303433001107</v>
+        <v>49.230343300110697</v>
       </c>
       <c r="H6">
-        <v>349.263736263736</v>
+        <v>349.26373626373601</v>
       </c>
       <c r="I6">
-        <v>4.39633699633699</v>
+        <v>4.3963369963369896</v>
       </c>
       <c r="K6">
         <v>502.5</v>
@@ -1571,10 +954,10 @@
         <v>587.3125</v>
       </c>
       <c r="O6">
-        <v>35.4475806451613</v>
-      </c>
-    </row>
-    <row r="7" ht="62.25" spans="3:4">
+        <v>35.447580645161302</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" ht="76.5">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -1582,7 +965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" ht="14.25" spans="2:15">
+    <row r="9" spans="2:26">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1590,25 +973,25 @@
         <v>12</v>
       </c>
       <c r="E9" s="16">
-        <v>276.232558139534</v>
+        <v>276.23255813953398</v>
       </c>
       <c r="F9">
-        <v>3.70653377630122</v>
+        <v>3.7065337763012201</v>
       </c>
       <c r="K9">
-        <v>534.739130434783</v>
+        <v>534.73913043478296</v>
       </c>
       <c r="L9">
-        <v>43.3526570048309</v>
+        <v>43.352657004830903</v>
       </c>
       <c r="N9">
-        <v>683.708333333333</v>
+        <v>683.70833333333303</v>
       </c>
       <c r="O9">
-        <v>135.69384057971</v>
-      </c>
-    </row>
-    <row r="10" ht="62.25" spans="3:4">
+        <v>135.69384057971001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" ht="91.5">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -1616,7 +999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" ht="14.25" spans="2:15">
+    <row r="12" spans="2:26">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -1624,31 +1007,31 @@
         <v>12</v>
       </c>
       <c r="E12" s="16">
-        <v>273.558139534883</v>
+        <v>273.55813953488303</v>
       </c>
       <c r="F12">
-        <v>9.20487264673312</v>
+        <v>9.2048726467331203</v>
       </c>
       <c r="H12" s="16">
         <v>317.622641509434</v>
       </c>
       <c r="I12">
-        <v>6.69433962264151</v>
+        <v>6.6943396226415102</v>
       </c>
       <c r="K12">
-        <v>483.95652173913</v>
+        <v>483.95652173912998</v>
       </c>
       <c r="L12">
-        <v>619.909178743961</v>
+        <v>619.90917874396098</v>
       </c>
       <c r="N12">
-        <v>661.583333333333</v>
+        <v>661.58333333333303</v>
       </c>
       <c r="O12">
-        <v>74.8785714285714</v>
-      </c>
-    </row>
-    <row r="13" ht="62.25" spans="3:4">
+        <v>74.878571428571405</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" ht="91.5">
       <c r="C13" t="s">
         <v>14</v>
       </c>
@@ -1656,7 +1039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" ht="14.25" spans="2:15">
+    <row r="15" spans="2:26">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1664,16 +1047,16 @@
         <v>12</v>
       </c>
       <c r="E15" s="16">
-        <v>289.976744186046</v>
+        <v>289.97674418604601</v>
       </c>
       <c r="F15">
         <v>12.9756367663344</v>
       </c>
       <c r="K15">
-        <v>471.239130434783</v>
+        <v>471.23913043478302</v>
       </c>
       <c r="L15">
-        <v>7.43043478260869</v>
+        <v>7.4304347826086898</v>
       </c>
       <c r="N15">
         <v>596.5625</v>
@@ -1682,7 +1065,7 @@
         <v>19.0625</v>
       </c>
     </row>
-    <row r="16" ht="62.25" spans="3:4">
+    <row r="16" spans="2:26" ht="76.5">
       <c r="C16" t="s">
         <v>14</v>
       </c>
@@ -1691,55 +1074,53 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AP16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.14166666666667" style="2"/>
-    <col min="4" max="4" width="2.14166666666667" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.425" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.425" style="2" customWidth="1"/>
-    <col min="7" max="7" width="3.56666666666667" style="2" customWidth="1"/>
-    <col min="8" max="9" width="9.14166666666667" style="2"/>
-    <col min="10" max="10" width="11.425" style="3"/>
-    <col min="11" max="11" width="9.14166666666667" style="3"/>
-    <col min="12" max="12" width="3.425" style="2" customWidth="1"/>
-    <col min="13" max="14" width="9.14166666666667" style="2"/>
-    <col min="15" max="16" width="9.14166666666667" style="3"/>
-    <col min="17" max="17" width="3.70833333333333" style="2" customWidth="1"/>
-    <col min="18" max="19" width="9.14166666666667" style="2"/>
-    <col min="20" max="21" width="9.14166666666667" style="3"/>
-    <col min="22" max="22" width="2.85833333333333" style="2" customWidth="1"/>
-    <col min="23" max="24" width="9.14166666666667" style="2"/>
-    <col min="25" max="26" width="9.14166666666667" style="3"/>
+    <col min="1" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="2.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="11.42578125" style="3"/>
+    <col min="11" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="3.42578125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="2"/>
+    <col min="15" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="3.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="2"/>
+    <col min="20" max="21" width="9.140625" style="3"/>
+    <col min="22" max="22" width="2.85546875" style="2" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" style="2"/>
+    <col min="25" max="26" width="9.140625" style="3"/>
     <col min="27" max="27" width="5" style="4" customWidth="1"/>
-    <col min="28" max="28" width="9.14166666666667" style="4"/>
-    <col min="29" max="29" width="9.14166666666667" style="2"/>
-    <col min="30" max="31" width="9.14166666666667" style="5"/>
+    <col min="28" max="28" width="9.140625" style="4"/>
+    <col min="29" max="29" width="9.140625" style="2"/>
+    <col min="30" max="31" width="9.140625" style="5"/>
     <col min="32" max="32" width="5" style="2" customWidth="1"/>
-    <col min="33" max="34" width="9.14166666666667" style="2"/>
-    <col min="35" max="36" width="9.14166666666667" style="5"/>
-    <col min="37" max="37" width="1.28333333333333" style="2" customWidth="1"/>
-    <col min="38" max="39" width="9.14166666666667" style="2"/>
-    <col min="40" max="40" width="1.14166666666667" style="2" customWidth="1"/>
-    <col min="41" max="41" width="9.14166666666667" style="6"/>
-    <col min="42" max="16384" width="9.14166666666667" style="2"/>
+    <col min="33" max="34" width="9.140625" style="2"/>
+    <col min="35" max="36" width="9.140625" style="5"/>
+    <col min="37" max="37" width="1.28515625" style="2" customWidth="1"/>
+    <col min="38" max="39" width="9.140625" style="2"/>
+    <col min="40" max="40" width="1.140625" style="2" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" style="6"/>
+    <col min="42" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:38">
+    <row r="1" spans="2:42">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +1149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:41">
+    <row r="2" spans="2:42">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1869,40 +1250,40 @@
         <v>12</v>
       </c>
       <c r="J3" s="3">
-        <v>333.603773584906</v>
+        <v>333.60377358490598</v>
       </c>
       <c r="K3" s="3">
-        <v>1.50703820741166</v>
+        <v>1.5070382074116599</v>
       </c>
       <c r="O3" s="3">
-        <v>434.447916666667</v>
+        <v>434.44791666666703</v>
       </c>
       <c r="P3" s="3">
-        <v>1.90121039515842</v>
+        <v>1.9012103951584201</v>
       </c>
       <c r="T3" s="3">
-        <v>533.493927125506</v>
+        <v>533.49392712550605</v>
       </c>
       <c r="U3" s="3">
-        <v>2.46693553719008</v>
+        <v>2.4669355371900799</v>
       </c>
       <c r="Y3" s="3">
-        <v>626.151898734177</v>
+        <v>626.15189873417705</v>
       </c>
       <c r="Z3" s="3">
-        <v>3.57167393314837</v>
+        <v>3.5716739331483698</v>
       </c>
       <c r="AD3" s="5">
-        <v>724.064377682404</v>
+        <v>724.06437768240403</v>
       </c>
       <c r="AE3" s="5">
         <v>1.87045512142037</v>
       </c>
       <c r="AI3" s="5">
-        <v>846.405247813411</v>
+        <v>846.40524781341105</v>
       </c>
       <c r="AJ3" s="5">
-        <v>4.13904561142454</v>
+        <v>4.1390456114245398</v>
       </c>
       <c r="AO3" s="6" t="s">
         <v>30</v>
@@ -1911,7 +1292,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" ht="16.5" spans="3:42">
+    <row r="4" spans="2:42" ht="16.5">
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1920,11 +1301,11 @@
       <c r="X4" s="4"/>
       <c r="AP4" s="6"/>
     </row>
-    <row r="5" spans="8:9">
+    <row r="5" spans="2:42">
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="2:36">
+    <row r="6" spans="2:42">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1933,53 +1314,53 @@
       </c>
       <c r="E6" s="10"/>
       <c r="J6" s="3">
-        <v>318.792452830189</v>
+        <v>318.79245283018901</v>
       </c>
       <c r="K6" s="3">
-        <v>2.61936225222637</v>
+        <v>2.6193622522263702</v>
       </c>
       <c r="O6" s="2">
-        <v>428.416666666667</v>
+        <v>428.41666666666703</v>
       </c>
       <c r="P6" s="3">
-        <v>8.1441794232823</v>
+        <v>8.1441794232822993</v>
       </c>
       <c r="T6" s="2">
-        <v>529.374545454546</v>
+        <v>529.37454545454602</v>
       </c>
       <c r="U6" s="3">
-        <v>2.57952163396936</v>
+        <v>2.5795216339693599</v>
       </c>
       <c r="Y6" s="2">
-        <v>624.740384615385</v>
+        <v>624.74038461538498</v>
       </c>
       <c r="Z6" s="3">
-        <v>4.24338585017836</v>
+        <v>4.2433858501783597</v>
       </c>
       <c r="AD6" s="5">
-        <v>718.655844155844</v>
+        <v>718.65584415584397</v>
       </c>
       <c r="AE6" s="5">
-        <v>2.83965397923876</v>
+        <v>2.8396539792387601</v>
       </c>
       <c r="AI6" s="5">
-        <v>820.031496062992</v>
+        <v>820.03149606299201</v>
       </c>
       <c r="AJ6" s="5">
-        <v>5.43433428901967</v>
-      </c>
-    </row>
-    <row r="7" ht="16.5" spans="3:4">
+        <v>5.4343342890196702</v>
+      </c>
+    </row>
+    <row r="7" spans="2:42" ht="16.5">
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="8:9">
+    <row r="8" spans="2:42">
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="2:36">
+    <row r="9" spans="2:42">
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1988,53 +1369,53 @@
       </c>
       <c r="E9" s="10"/>
       <c r="J9" s="3">
-        <v>322.584905660377</v>
+        <v>322.58490566037699</v>
       </c>
       <c r="K9" s="3">
-        <v>1.22263717322609</v>
+        <v>1.2226371732260899</v>
       </c>
       <c r="O9" s="3">
         <v>433.96875</v>
       </c>
       <c r="P9" s="3">
-        <v>1.50943396226415</v>
+        <v>1.5094339622641499</v>
       </c>
       <c r="T9" s="3">
         <v>539.638783269962</v>
       </c>
       <c r="U9" s="3">
-        <v>1.46692448368648</v>
+        <v>1.4669244836864801</v>
       </c>
       <c r="Y9" s="3">
-        <v>631.833333333333</v>
+        <v>631.83333333333303</v>
       </c>
       <c r="Z9" s="3">
-        <v>3.43603814801002</v>
+        <v>3.4360381480100202</v>
       </c>
       <c r="AD9" s="5">
-        <v>718.249011857708</v>
+        <v>718.24901185770796</v>
       </c>
       <c r="AE9" s="5">
         <v>2.39381466800066</v>
       </c>
       <c r="AI9" s="5">
-        <v>838.077639751553</v>
+        <v>838.07763975155297</v>
       </c>
       <c r="AJ9" s="5">
-        <v>3.70796791610749</v>
-      </c>
-    </row>
-    <row r="10" ht="16.5" spans="3:4">
+        <v>3.7079679161074899</v>
+      </c>
+    </row>
+    <row r="10" spans="2:42" ht="16.5">
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="8:9">
+    <row r="11" spans="2:42">
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="2:36">
+    <row r="12" spans="2:42">
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2043,53 +1424,53 @@
       </c>
       <c r="E12" s="10"/>
       <c r="J12" s="3">
-        <v>352.117647058824</v>
+        <v>352.11764705882399</v>
       </c>
       <c r="K12" s="3">
-        <v>4.72329947676208</v>
+        <v>4.7232994767620804</v>
       </c>
       <c r="O12" s="3">
-        <v>467.354166666667</v>
+        <v>467.35416666666703</v>
       </c>
       <c r="P12" s="3">
-        <v>3.63011747953008</v>
+        <v>3.6301174795300799</v>
       </c>
       <c r="T12" s="3">
-        <v>523.479853479853</v>
+        <v>523.47985347985298</v>
       </c>
       <c r="U12" s="3">
-        <v>2.43945582677079</v>
+        <v>2.4394558267707902</v>
       </c>
       <c r="Y12" s="3">
-        <v>627.411764705882</v>
+        <v>627.41176470588198</v>
       </c>
       <c r="Z12" s="3">
         <v>8.30193909275933</v>
       </c>
       <c r="AD12" s="5">
-        <v>744.07874015748</v>
+        <v>744.07874015747996</v>
       </c>
       <c r="AE12" s="5">
         <v>2.62091947085157</v>
       </c>
       <c r="AI12" s="5">
-        <v>858.652421652422</v>
+        <v>858.65242165242205</v>
       </c>
       <c r="AJ12" s="5">
-        <v>7.21756137126261</v>
-      </c>
-    </row>
-    <row r="13" ht="16.5" spans="3:4">
+        <v>7.2175613712626099</v>
+      </c>
+    </row>
+    <row r="13" spans="2:42" ht="16.5">
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="8:9">
+    <row r="14" spans="2:42">
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="2:36">
+    <row r="15" spans="2:42">
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2098,98 +1479,96 @@
       </c>
       <c r="E15" s="10"/>
       <c r="J15" s="3">
-        <v>322.22641509434</v>
+        <v>322.22641509433998</v>
       </c>
       <c r="K15" s="3">
-        <v>1.48750359092215</v>
+        <v>1.4875035909221499</v>
       </c>
       <c r="O15" s="3">
-        <v>419.572916666667</v>
+        <v>419.57291666666703</v>
       </c>
       <c r="P15" s="3">
         <v>1.82912068351727</v>
       </c>
       <c r="T15" s="3">
-        <v>510.621621621622</v>
+        <v>510.62162162162201</v>
       </c>
       <c r="U15" s="3">
         <v>2.95508625817966</v>
       </c>
       <c r="Y15" s="3">
-        <v>616.188976377953</v>
+        <v>616.18897637795305</v>
       </c>
       <c r="Z15" s="3">
-        <v>4.47220964740205</v>
+        <v>4.4722096474020496</v>
       </c>
       <c r="AD15" s="5">
         <v>707.2578125</v>
       </c>
       <c r="AE15" s="5">
-        <v>2.55613965483038</v>
+        <v>2.5561396548303801</v>
       </c>
       <c r="AI15" s="5">
-        <v>825.232258064516</v>
+        <v>825.23225806451603</v>
       </c>
       <c r="AJ15" s="5">
-        <v>4.51521935246751</v>
-      </c>
-    </row>
-    <row r="16" ht="16.5" spans="3:4">
+        <v>4.5152193524675104</v>
+      </c>
+    </row>
+    <row r="16" spans="2:42" ht="16.5">
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AP41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AO10" sqref="AO10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="2" customWidth="1"/>
-    <col min="2" max="3" width="9.14166666666667" style="2"/>
-    <col min="4" max="4" width="2.14166666666667" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.425" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.425" style="2" customWidth="1"/>
-    <col min="7" max="7" width="3.56666666666667" style="2" customWidth="1"/>
-    <col min="8" max="9" width="9.14166666666667" style="2"/>
-    <col min="10" max="11" width="9.14166666666667" style="3"/>
-    <col min="12" max="12" width="3.425" style="2" customWidth="1"/>
-    <col min="13" max="14" width="9.14166666666667" style="2"/>
-    <col min="15" max="16" width="9.14166666666667" style="3"/>
-    <col min="17" max="17" width="1.28333333333333" style="2" customWidth="1"/>
-    <col min="18" max="19" width="9.14166666666667" style="2"/>
-    <col min="20" max="21" width="9.14166666666667" style="3"/>
-    <col min="22" max="22" width="2.85833333333333" style="2" customWidth="1"/>
-    <col min="23" max="24" width="9.14166666666667" style="2"/>
-    <col min="25" max="26" width="9.14166666666667" style="3"/>
-    <col min="27" max="27" width="2.425" style="4" customWidth="1"/>
-    <col min="28" max="28" width="9.14166666666667" style="4"/>
-    <col min="29" max="29" width="9.14166666666667" style="2"/>
-    <col min="30" max="31" width="9.14166666666667" style="5"/>
-    <col min="32" max="32" width="1.70833333333333" style="2" customWidth="1"/>
-    <col min="33" max="34" width="9.14166666666667" style="2"/>
-    <col min="35" max="36" width="9.14166666666667" style="5"/>
-    <col min="37" max="37" width="1.28333333333333" style="2" customWidth="1"/>
-    <col min="38" max="39" width="9.14166666666667" style="2"/>
-    <col min="40" max="40" width="3.28333333333333" style="2" customWidth="1"/>
-    <col min="41" max="41" width="9.14166666666667" style="6"/>
-    <col min="42" max="16384" width="9.14166666666667" style="2"/>
+    <col min="2" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="2.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="2"/>
+    <col min="10" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="3.42578125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="2"/>
+    <col min="15" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="1.28515625" style="2" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="2"/>
+    <col min="20" max="21" width="9.140625" style="3"/>
+    <col min="22" max="22" width="2.85546875" style="2" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" style="2"/>
+    <col min="25" max="26" width="9.140625" style="3"/>
+    <col min="27" max="27" width="2.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="4"/>
+    <col min="29" max="29" width="9.140625" style="2"/>
+    <col min="30" max="31" width="9.140625" style="5"/>
+    <col min="32" max="32" width="1.7109375" style="2" customWidth="1"/>
+    <col min="33" max="34" width="9.140625" style="2"/>
+    <col min="35" max="36" width="9.140625" style="5"/>
+    <col min="37" max="37" width="1.28515625" style="2" customWidth="1"/>
+    <col min="38" max="39" width="9.140625" style="2"/>
+    <col min="40" max="40" width="3.28515625" style="2" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" style="6"/>
+    <col min="42" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:41">
+    <row r="1" spans="2:42">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2325,43 +1704,43 @@
         <v>12</v>
       </c>
       <c r="J3" s="3">
-        <v>3158.83333333333</v>
+        <v>3158.8333333333298</v>
       </c>
       <c r="K3" s="3">
-        <v>35.2456574394463</v>
+        <v>35.245657439446298</v>
       </c>
       <c r="O3" s="3">
-        <v>4237.25222551929</v>
+        <v>4237.2522255192898</v>
       </c>
       <c r="P3" s="3">
-        <v>17.6589226666667</v>
+        <v>17.658922666666701</v>
       </c>
       <c r="T3" s="3">
-        <v>5428.47858942066</v>
+        <v>5428.4785894206598</v>
       </c>
       <c r="U3" s="3">
-        <v>23.1500557895116</v>
+        <v>23.150055789511601</v>
       </c>
       <c r="Y3" s="3">
-        <v>6453.11788617886</v>
+        <v>6453.1178861788603</v>
       </c>
       <c r="Z3" s="3">
         <v>27.2390838786438</v>
       </c>
       <c r="AI3" s="5">
-        <v>8251.85582010582</v>
+        <v>8251.8558201058204</v>
       </c>
       <c r="AJ3" s="5">
-        <v>38.2388500921202</v>
+        <v>38.238850092120202</v>
       </c>
       <c r="AO3" s="6">
-        <v>0.9734</v>
+        <v>0.97340000000000004</v>
       </c>
       <c r="AP3" s="2">
         <v>-159.5</v>
       </c>
     </row>
-    <row r="4" ht="16.5" spans="3:42">
+    <row r="4" spans="2:42" ht="16.5">
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
@@ -2370,7 +1749,7 @@
       <c r="X4" s="4"/>
       <c r="AP4" s="6"/>
     </row>
-    <row r="5" spans="8:9">
+    <row r="5" spans="2:42">
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
@@ -2383,7 +1762,7 @@
       </c>
       <c r="E6" s="10"/>
       <c r="J6" s="3">
-        <v>3235.05586942875</v>
+        <v>3235.0558694287502</v>
       </c>
       <c r="K6" s="3">
         <v>20.6112700692651</v>
@@ -2392,28 +1771,28 @@
         <v>32</v>
       </c>
       <c r="O6" s="2">
-        <v>4101.38095238095</v>
+        <v>4101.3809523809496</v>
       </c>
       <c r="P6" s="3">
         <v>24.9340587524099</v>
       </c>
       <c r="T6" s="2">
-        <v>5217.82962962963</v>
+        <v>5217.8296296296303</v>
       </c>
       <c r="U6" s="3">
-        <v>22.452377323612</v>
+        <v>22.452377323612001</v>
       </c>
       <c r="Y6" s="2">
-        <v>5919.39164370983</v>
+        <v>5919.3916437098296</v>
       </c>
       <c r="Z6" s="3">
-        <v>30.0226901623314</v>
+        <v>30.022690162331401</v>
       </c>
       <c r="AI6" s="5">
-        <v>8081.34496996997</v>
+        <v>8081.3449699699704</v>
       </c>
       <c r="AJ6" s="5">
-        <v>25.5073933984663</v>
+        <v>25.507393398466299</v>
       </c>
       <c r="AN6" s="9">
         <v>1</v>
@@ -2425,19 +1804,19 @@
         <v>-291.3</v>
       </c>
     </row>
-    <row r="7" ht="16.5" spans="3:42">
+    <row r="7" spans="2:42" ht="16.5">
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="N7" s="2">
+      <c r="N7" s="9">
         <v>1</v>
       </c>
       <c r="O7" s="3">
         <v>4109.42565597668</v>
       </c>
       <c r="P7" s="3">
-        <v>25.9468314492184</v>
+        <v>25.946831449218401</v>
       </c>
       <c r="AN7" s="2">
         <v>2</v>
@@ -2446,17 +1825,17 @@
         <v>1.032</v>
       </c>
       <c r="AP7" s="2">
-        <v>-276.4</v>
-      </c>
-    </row>
-    <row r="8" spans="8:42">
+        <v>-276.39999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:42">
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
       <c r="O8" s="3">
-        <v>4088.33497536946</v>
+        <v>4088.3349753694602</v>
       </c>
       <c r="P8" s="3">
         <v>19.5649185185185</v>
@@ -2465,10 +1844,10 @@
         <v>32</v>
       </c>
       <c r="AO8" s="6">
-        <v>1.033</v>
+        <v>1.0329999999999999</v>
       </c>
       <c r="AP8" s="2">
-        <v>-285.6</v>
+        <v>-285.60000000000002</v>
       </c>
     </row>
     <row r="9" spans="2:42">
@@ -2480,49 +1859,49 @@
       </c>
       <c r="E9" s="10"/>
       <c r="J9" s="3">
-        <v>3337.36094674556</v>
+        <v>3337.3609467455599</v>
       </c>
       <c r="K9" s="3">
         <v>14.7810943866003</v>
       </c>
       <c r="O9" s="3">
-        <v>4308.78734177215</v>
+        <v>4308.7873417721503</v>
       </c>
       <c r="P9" s="3">
         <v>28.318761318175</v>
       </c>
       <c r="T9" s="3">
-        <v>5137.60891089109</v>
+        <v>5137.6089108910901</v>
       </c>
       <c r="U9" s="3">
-        <v>20.1601961096939</v>
+        <v>20.160196109693899</v>
       </c>
       <c r="Y9" s="3">
-        <v>6208.8702435312</v>
+        <v>6208.8702435311998</v>
       </c>
       <c r="Z9" s="3">
-        <v>24.999786545318</v>
+        <v>24.999786545317999</v>
       </c>
       <c r="AI9" s="5">
-        <v>8390.27577216206</v>
+        <v>8390.2757721620601</v>
       </c>
       <c r="AJ9" s="5">
         <v>60.5598701924986</v>
       </c>
       <c r="AO9" s="6">
-        <v>0.9893</v>
+        <v>0.98929999999999996</v>
       </c>
       <c r="AP9" s="2">
         <v>-218.1</v>
       </c>
     </row>
-    <row r="10" ht="16.5" spans="3:4">
+    <row r="10" spans="2:42" ht="16.5">
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="8:9">
+    <row r="11" spans="2:42">
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
@@ -2535,34 +1914,34 @@
       </c>
       <c r="E12" s="10"/>
       <c r="J12" s="3">
-        <v>3274.36011904762</v>
+        <v>3274.3601190476202</v>
       </c>
       <c r="K12" s="3">
-        <v>13.7975635562927</v>
+        <v>13.797563556292699</v>
       </c>
       <c r="O12" s="3">
-        <v>4701.51351351351</v>
+        <v>4701.5135135135097</v>
       </c>
       <c r="P12" s="3">
-        <v>19.7969609506393</v>
+        <v>19.796960950639299</v>
       </c>
       <c r="T12" s="3">
-        <v>5407.78325123153</v>
+        <v>5407.7832512315299</v>
       </c>
       <c r="U12" s="3">
         <v>23.5817507244107</v>
       </c>
       <c r="Y12" s="3">
-        <v>6566.58201058201</v>
+        <v>6566.5820105820103</v>
       </c>
       <c r="Z12" s="3">
-        <v>32.8796825396825</v>
+        <v>32.879682539682499</v>
       </c>
       <c r="AI12" s="5">
-        <v>8048.37884914464</v>
+        <v>8048.3788491446403</v>
       </c>
       <c r="AJ12" s="5">
-        <v>36.3142070449019</v>
+        <v>36.314207044901899</v>
       </c>
       <c r="AO12" s="6">
         <v>1.052</v>
@@ -2571,13 +1950,13 @@
         <v>-688.6</v>
       </c>
     </row>
-    <row r="13" ht="16.5" spans="3:4">
+    <row r="13" spans="2:42" ht="16.5">
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="8:9">
+    <row r="14" spans="2:42">
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
     </row>
@@ -2590,43 +1969,43 @@
       </c>
       <c r="E15" s="10"/>
       <c r="J15" s="3">
-        <v>3187.37350119904</v>
+        <v>3187.3735011990402</v>
       </c>
       <c r="K15" s="3">
-        <v>27.3274638993844</v>
+        <v>27.327463899384401</v>
       </c>
       <c r="O15" s="3">
-        <v>4300.88148148148</v>
+        <v>4300.8814814814796</v>
       </c>
       <c r="P15" s="3">
-        <v>24.9543206630919</v>
+        <v>24.954320663091899</v>
       </c>
       <c r="T15" s="3">
-        <v>5367.57046979866</v>
+        <v>5367.5704697986603</v>
       </c>
       <c r="U15" s="3">
-        <v>23.8170592974345</v>
+        <v>23.817059297434501</v>
       </c>
       <c r="Y15" s="3">
-        <v>6237.76911314985</v>
+        <v>6237.7691131498505</v>
       </c>
       <c r="Z15" s="3">
         <v>19.6181020116152</v>
       </c>
       <c r="AI15" s="5">
-        <v>8135.18888888889</v>
+        <v>8135.1888888888898</v>
       </c>
       <c r="AJ15" s="5">
-        <v>43.8301806094172</v>
+        <v>43.830180609417198</v>
       </c>
       <c r="AO15" s="6">
-        <v>1.017</v>
+        <v>1.0169999999999999</v>
       </c>
       <c r="AP15" s="2">
         <v>-339</v>
       </c>
     </row>
-    <row r="16" ht="16.5" spans="3:15">
+    <row r="16" spans="2:42" ht="16.5">
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2645,10 +2024,10 @@
         <v>34</v>
       </c>
       <c r="J18" s="3">
-        <v>3445.12881464825</v>
+        <v>3445.1288146482502</v>
       </c>
       <c r="K18" s="3">
-        <v>16.5636063343433</v>
+        <v>16.563606334343302</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>35</v>
@@ -2657,19 +2036,19 @@
         <v>36</v>
       </c>
       <c r="T18" s="3">
-        <v>5582.21234567901</v>
+        <v>5582.2123456790096</v>
       </c>
       <c r="U18" s="3">
         <v>19.8668541452599</v>
       </c>
       <c r="Y18" s="3">
-        <v>6282.34305150632</v>
+        <v>6282.3430515063201</v>
       </c>
       <c r="Z18" s="3">
-        <v>17.2493996549055</v>
+        <v>17.249399654905499</v>
       </c>
       <c r="AI18" s="5">
-        <v>8132.49187725632</v>
+        <v>8132.4918772563196</v>
       </c>
       <c r="AJ18" s="5">
         <v>28.5014857845756</v>
@@ -2678,13 +2057,13 @@
         <v>1</v>
       </c>
       <c r="AO18" s="11">
-        <v>1.074</v>
+        <v>1.0740000000000001</v>
       </c>
       <c r="AP18" s="9">
         <v>-796.4</v>
       </c>
     </row>
-    <row r="19" ht="16.5" spans="3:42">
+    <row r="19" spans="2:42" ht="16.5">
       <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
@@ -2693,104 +2072,104 @@
         <v>37</v>
       </c>
       <c r="J19" s="3">
-        <v>3327.86842105263</v>
+        <v>3333.8056994818699</v>
       </c>
       <c r="K19" s="3">
-        <v>98.733560090703</v>
-      </c>
-      <c r="N19" s="2">
+        <v>132.316796226744</v>
+      </c>
+      <c r="N19" s="9">
         <v>1</v>
       </c>
       <c r="O19" s="2">
-        <v>4476.08374384236</v>
+        <v>4476.0837438423596</v>
       </c>
       <c r="P19" s="3">
-        <v>26.092187654321</v>
+        <v>26.092187654320998</v>
       </c>
       <c r="AN19" s="2">
         <v>2</v>
       </c>
       <c r="AO19" s="6">
-        <v>1.092</v>
+        <v>1.0920000000000001</v>
       </c>
       <c r="AP19" s="2">
         <v>-946.9</v>
       </c>
     </row>
-    <row r="20" spans="14:16">
+    <row r="20" spans="2:42">
       <c r="N20" s="2">
         <v>2</v>
       </c>
       <c r="O20" s="3">
-        <v>4702.56976744186</v>
+        <v>4702.5697674418598</v>
       </c>
       <c r="P20" s="3">
-        <v>36.951135734072</v>
-      </c>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="41:41">
+        <v>36.951135734071997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:42" s="1" customFormat="1">
       <c r="AO22" s="12"/>
     </row>
-    <row r="26" spans="12:14">
+    <row r="26" spans="2:42">
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="12:14">
+    <row r="27" spans="2:42">
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="12:14">
+    <row r="28" spans="2:42">
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="11:14">
+    <row r="29" spans="2:42">
       <c r="K29" s="2"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="12:14">
+    <row r="30" spans="2:42">
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="12:14">
+    <row r="31" spans="2:42">
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="12:14">
+    <row r="32" spans="2:42">
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="12:14">
+    <row r="33" spans="11:14">
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="12:14">
+    <row r="34" spans="11:14">
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="12:14">
+    <row r="35" spans="11:14">
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="12:14">
+    <row r="36" spans="11:14">
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="12:14">
+    <row r="37" spans="11:14">
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="12:14">
+    <row r="38" spans="11:14">
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="5"/>
@@ -2801,7 +2180,7 @@
       <c r="M39" s="3"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="12:14">
+    <row r="40" spans="11:14">
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="5"/>
@@ -2813,7 +2192,6 @@
       <c r="N41" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change legend in '\forAlignment\forAlignment.m'. reflection in 'RotationTranslationComparison.m' works
</commit_message>
<xml_diff>
--- a/communicate_with_basis_station_in_matlab/calibrations/outdoor/OUTDOOR_MEASUREMENT_07_27_2017/outdoor_calibration_results.xlsx
+++ b/communicate_with_basis_station_in_matlab/calibrations/outdoor/OUTDOOR_MEASUREMENT_07_27_2017/outdoor_calibration_results.xlsx
@@ -329,9 +329,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -359,6 +359,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -366,7 +373,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,15 +396,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -405,28 +412,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -440,9 +425,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,40 +442,9 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -503,6 +464,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -514,7 +514,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,6 +559,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -571,7 +715,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,163 +727,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,44 +788,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -852,16 +811,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -880,151 +848,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2165,10 +2159,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:AP44"/>
+  <dimension ref="B1:AP41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5"/>
@@ -2183,14 +2177,14 @@
     <col min="10" max="11" width="9.14166666666667" style="3"/>
     <col min="12" max="12" width="3.425" style="2" customWidth="1"/>
     <col min="13" max="14" width="9.14166666666667" style="2"/>
-    <col min="15" max="16" width="9.14166666666667" style="3"/>
+    <col min="15" max="16" width="12.625" style="3"/>
     <col min="17" max="17" width="1.28333333333333" style="2" customWidth="1"/>
-    <col min="18" max="19" width="9.14166666666667" style="2"/>
-    <col min="20" max="21" width="9.14166666666667" style="3"/>
-    <col min="22" max="22" width="2.85833333333333" style="2" customWidth="1"/>
+    <col min="18" max="19" width="12.625" style="2"/>
+    <col min="20" max="21" width="12.625" style="3"/>
+    <col min="22" max="22" width="6" style="2" customWidth="1"/>
     <col min="23" max="23" width="12.625" style="2"/>
     <col min="24" max="24" width="9.14166666666667" style="2"/>
-    <col min="25" max="26" width="9.14166666666667" style="3"/>
+    <col min="25" max="26" width="12.625" style="3"/>
     <col min="27" max="27" width="2.425" style="4" customWidth="1"/>
     <col min="28" max="28" width="9.14166666666667" style="4"/>
     <col min="29" max="29" width="9.14166666666667" style="2"/>
@@ -2747,35 +2741,50 @@
     <row r="22" s="1" customFormat="1" spans="41:41">
       <c r="AO22" s="12"/>
     </row>
-    <row r="26" spans="12:14">
+    <row r="26" spans="12:23">
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="5"/>
-    </row>
-    <row r="27" spans="12:23">
+      <c r="R26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="12:22">
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="5"/>
       <c r="P27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="R27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V27" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W27" s="2" t="s">
-        <v>9</v>
+      <c r="R27" s="2">
+        <v>3</v>
+      </c>
+      <c r="S27" s="2">
+        <v>4</v>
+      </c>
+      <c r="T27" s="3">
+        <v>5</v>
+      </c>
+      <c r="U27" s="3">
+        <v>6</v>
+      </c>
+      <c r="V27" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="12:23">
@@ -2802,203 +2811,167 @@
         <v>28.3065139732777</v>
       </c>
     </row>
-    <row r="29" spans="11:22">
+    <row r="29" spans="11:23">
       <c r="K29" s="2"/>
       <c r="N29" s="5"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="V29" s="5"/>
-    </row>
-    <row r="30" spans="12:22">
+      <c r="R29" s="3">
+        <v>20.6112700692651</v>
+      </c>
+      <c r="S29" s="3">
+        <v>24.9340587524099</v>
+      </c>
+      <c r="T29" s="3">
+        <v>22.452377323612</v>
+      </c>
+      <c r="U29" s="3">
+        <v>30.0226901623314</v>
+      </c>
+      <c r="V29" s="5">
+        <v>25.5073933984663</v>
+      </c>
+      <c r="W29" s="2">
+        <f>AVERAGE(R29,S29,T29,U29,V29)</f>
+        <v>24.7055579412169</v>
+      </c>
+    </row>
+    <row r="30" spans="12:23">
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="5"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="V30" s="5"/>
+      <c r="R30" s="3">
+        <v>14.7810943866003</v>
+      </c>
+      <c r="S30" s="3">
+        <v>28.318761318175</v>
+      </c>
+      <c r="T30" s="3">
+        <v>20.1601961096939</v>
+      </c>
+      <c r="U30" s="3">
+        <v>24.999786545318</v>
+      </c>
+      <c r="V30" s="5">
+        <v>60.5598701924986</v>
+      </c>
+      <c r="W30" s="2">
+        <f>AVERAGE(R30,S30,T30,U30,V30)</f>
+        <v>29.7639417104572</v>
+      </c>
     </row>
     <row r="31" spans="12:23">
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="5"/>
       <c r="R31" s="3">
-        <v>20.6112700692651</v>
+        <v>13.7975635562927</v>
       </c>
       <c r="S31" s="3">
-        <v>24.9340587524099</v>
+        <v>19.7969609506393</v>
       </c>
       <c r="T31" s="3">
-        <v>22.452377323612</v>
+        <v>23.5817507244107</v>
       </c>
       <c r="U31" s="3">
-        <v>30.0226901623314</v>
+        <v>32.8796825396825</v>
       </c>
       <c r="V31" s="5">
-        <v>25.5073933984663</v>
+        <v>36.3142070449019</v>
       </c>
       <c r="W31" s="2">
         <f>AVERAGE(R31,S31,T31,U31,V31)</f>
-        <v>24.7055579412169</v>
-      </c>
-    </row>
-    <row r="32" spans="12:22">
+        <v>25.2740329631854</v>
+      </c>
+    </row>
+    <row r="32" spans="12:23">
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="5"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="V32" s="5"/>
-    </row>
-    <row r="33" spans="12:22">
+      <c r="R32" s="3">
+        <v>27.3274638993844</v>
+      </c>
+      <c r="S32" s="3">
+        <v>24.9543206630919</v>
+      </c>
+      <c r="T32" s="3">
+        <v>23.8170592974345</v>
+      </c>
+      <c r="U32" s="3">
+        <v>19.6181020116152</v>
+      </c>
+      <c r="V32" s="5">
+        <v>43.8301806094172</v>
+      </c>
+      <c r="W32" s="2">
+        <f>AVERAGE(R32,S32,T32,U32,V32)</f>
+        <v>27.9094252961886</v>
+      </c>
+    </row>
+    <row r="33" spans="12:23">
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="5"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="V33" s="5"/>
-    </row>
-    <row r="34" spans="12:23">
+      <c r="R33" s="3">
+        <v>16.5636063343433</v>
+      </c>
+      <c r="S33" s="3">
+        <v>26.092187654321</v>
+      </c>
+      <c r="T33" s="3">
+        <v>19.8668541452599</v>
+      </c>
+      <c r="U33" s="3">
+        <v>17.2493996549055</v>
+      </c>
+      <c r="V33" s="5">
+        <v>28.5014857845756</v>
+      </c>
+      <c r="W33" s="2">
+        <f>AVERAGE(R33,S33,T33,U33,V33)</f>
+        <v>21.6547067146811</v>
+      </c>
+    </row>
+    <row r="34" spans="12:19">
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="5"/>
-      <c r="R34" s="3">
-        <v>14.7810943866003</v>
-      </c>
-      <c r="S34" s="3">
-        <v>28.318761318175</v>
-      </c>
-      <c r="T34" s="3">
-        <v>20.1601961096939</v>
-      </c>
-      <c r="U34" s="3">
-        <v>24.999786545318</v>
-      </c>
-      <c r="V34" s="5">
-        <v>60.5598701924986</v>
-      </c>
-      <c r="W34" s="2">
-        <f>AVERAGE(R34,S34,T34,U34,V34)</f>
-        <v>29.7639417104572</v>
-      </c>
-    </row>
-    <row r="35" spans="12:22">
+      <c r="S34" s="3"/>
+    </row>
+    <row r="35" spans="12:14">
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="5"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="12:22">
+    </row>
+    <row r="36" spans="12:14">
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="5"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="V36" s="5"/>
-    </row>
-    <row r="37" spans="12:23">
+    </row>
+    <row r="37" spans="12:14">
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="5"/>
-      <c r="R37" s="3">
-        <v>13.7975635562927</v>
-      </c>
-      <c r="S37" s="3">
-        <v>19.7969609506393</v>
-      </c>
-      <c r="T37" s="3">
-        <v>23.5817507244107</v>
-      </c>
-      <c r="U37" s="3">
-        <v>32.8796825396825</v>
-      </c>
-      <c r="V37" s="5">
-        <v>36.3142070449019</v>
-      </c>
-      <c r="W37" s="2">
-        <f>AVERAGE(R37,S37,T37,U37,V37)</f>
-        <v>25.2740329631854</v>
-      </c>
-    </row>
-    <row r="38" spans="12:22">
+    </row>
+    <row r="38" spans="12:14">
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="5"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="V38" s="5"/>
-    </row>
-    <row r="39" spans="11:22">
+    </row>
+    <row r="39" spans="11:14">
       <c r="K39" s="2"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="5"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="V39" s="5"/>
-    </row>
-    <row r="40" spans="12:23">
+    </row>
+    <row r="40" spans="12:14">
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="5"/>
-      <c r="R40" s="3">
-        <v>27.3274638993844</v>
-      </c>
-      <c r="S40" s="3">
-        <v>24.9543206630919</v>
-      </c>
-      <c r="T40" s="3">
-        <v>23.8170592974345</v>
-      </c>
-      <c r="U40" s="3">
-        <v>19.6181020116152</v>
-      </c>
-      <c r="V40" s="5">
-        <v>43.8301806094172</v>
-      </c>
-      <c r="W40" s="2">
-        <f>AVERAGE(R40,S40,T40,U40,V40)</f>
-        <v>27.9094252961886</v>
-      </c>
-    </row>
-    <row r="41" spans="11:22">
+    </row>
+    <row r="41" spans="11:14">
       <c r="K41" s="2"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="5"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="V41" s="5"/>
-    </row>
-    <row r="42" spans="18:22">
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="V42" s="5"/>
-    </row>
-    <row r="43" spans="18:23">
-      <c r="R43" s="3">
-        <v>16.5636063343433</v>
-      </c>
-      <c r="S43" s="3">
-        <v>26.092187654321</v>
-      </c>
-      <c r="T43" s="3">
-        <v>19.8668541452599</v>
-      </c>
-      <c r="U43" s="3">
-        <v>17.2493996549055</v>
-      </c>
-      <c r="V43" s="5">
-        <v>28.5014857845756</v>
-      </c>
-      <c r="W43" s="2">
-        <f>AVERAGE(R43,S43,T43,U43,V43)</f>
-        <v>21.6547067146811</v>
-      </c>
-    </row>
-    <row r="44" spans="19:19">
-      <c r="S44" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.3" footer="0.3"/>

</xml_diff>